<commit_message>
Act greficos y tablas web pob
</commit_message>
<xml_diff>
--- a/indicadores/tablas/pob/130101_edad.xlsx
+++ b/indicadores/tablas/pob/130101_edad.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Datos" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Ficha técnica" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -60,100 +60,109 @@
     <t xml:space="preserve">17</t>
   </si>
   <si>
+    <t xml:space="preserve">2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2007</t>
+  </si>
+  <si>
     <t xml:space="preserve">2006</t>
   </si>
   <si>
-    <t xml:space="preserve">2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019</t>
-  </si>
-  <si>
     <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">DERECHO</t>
+    <t xml:space="preserve">nomindicador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porcentaje de personas de 4 a 17 años que no asisten a centros educativos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">derecho</t>
   </si>
   <si>
     <t xml:space="preserve">Educación</t>
   </si>
   <si>
-    <t xml:space="preserve">CONINDICADOR</t>
+    <t xml:space="preserve">conindicador</t>
   </si>
   <si>
     <t xml:space="preserve">No asistencia a centros educativos (4 a 17 años)</t>
   </si>
   <si>
-    <t xml:space="preserve">NOMINDICADOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porcentaje de personas de 4 a 17 años que no asisten a centros educativos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEFINICIÓN</t>
+    <t xml:space="preserve">tipoind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">definicion</t>
   </si>
   <si>
     <t xml:space="preserve">El indicador mide el porcentaje de personas de 4 a 17 años que no asisten a centros educativos.</t>
   </si>
   <si>
-    <t xml:space="preserve">CÁLCULO</t>
+    <t xml:space="preserve">calculo</t>
   </si>
   <si>
     <t xml:space="preserve">Para cada año calcular: (Cantidad de niños de 4 a 17 años que no asisten a centros educativos / Cantidad de población de 4 a 17 años)*100</t>
   </si>
   <si>
-    <t xml:space="preserve">TIPOIND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resultados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CITA</t>
+    <t xml:space="preserve">observaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin observaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cita</t>
   </si>
   <si>
     <t xml:space="preserve">UMAD con base en Instituto de Economía, Universidad de la República (2020) Encuesta Continua de Hogares Compatibilizada 1981-2018 Versión 12 DOI: http://doiorg/1047426/ECHINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirador DESCA - UMAD/FCS – INDDHH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -472,12 +481,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -531,46 +540,46 @@
         <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>23.5</v>
+        <v>5.8</v>
       </c>
       <c r="C2" t="n">
-        <v>4.8</v>
+        <v>0.64</v>
       </c>
       <c r="D2" t="n">
-        <v>0.71</v>
+        <v>1.1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.42</v>
+        <v>0.35</v>
       </c>
       <c r="F2" t="n">
-        <v>0.23</v>
+        <v>0.16</v>
       </c>
       <c r="G2" t="n">
-        <v>0.21</v>
+        <v>0.43</v>
       </c>
       <c r="H2" t="n">
-        <v>0.42</v>
+        <v>1.1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.45</v>
+        <v>1.1</v>
       </c>
       <c r="J2" t="n">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="K2" t="n">
-        <v>4.8</v>
+        <v>1.3</v>
       </c>
       <c r="L2" t="n">
-        <v>9.8</v>
+        <v>3.2</v>
       </c>
       <c r="M2" t="n">
-        <v>17.9</v>
+        <v>5.2</v>
       </c>
       <c r="N2" t="n">
-        <v>23.4</v>
+        <v>10</v>
       </c>
       <c r="O2" t="n">
-        <v>33.1</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="3">
@@ -578,46 +587,46 @@
         <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>21.1</v>
+        <v>6.5</v>
       </c>
       <c r="C3" t="n">
-        <v>5.3</v>
+        <v>0.99</v>
       </c>
       <c r="D3" t="n">
-        <v>0.66</v>
+        <v>0.71</v>
       </c>
       <c r="E3" t="n">
-        <v>0.46</v>
+        <v>0.18</v>
       </c>
       <c r="F3" t="n">
-        <v>0.34</v>
+        <v>0.22</v>
       </c>
       <c r="G3" t="n">
-        <v>0.082</v>
+        <v>0.076</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2</v>
+        <v>0.58</v>
       </c>
       <c r="I3" t="n">
-        <v>0.14</v>
+        <v>1.3</v>
       </c>
       <c r="J3" t="n">
         <v>1.2</v>
       </c>
       <c r="K3" t="n">
-        <v>5</v>
+        <v>2.6</v>
       </c>
       <c r="L3" t="n">
-        <v>11.3</v>
+        <v>3.8</v>
       </c>
       <c r="M3" t="n">
-        <v>17.9</v>
+        <v>6.5</v>
       </c>
       <c r="N3" t="n">
-        <v>25.4</v>
+        <v>12.7</v>
       </c>
       <c r="O3" t="n">
-        <v>34.5</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="4">
@@ -625,46 +634,46 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>19</v>
+        <v>6.6</v>
       </c>
       <c r="C4" t="n">
-        <v>3.7</v>
+        <v>0.99</v>
       </c>
       <c r="D4" t="n">
-        <v>1.1</v>
+        <v>0.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.84</v>
+        <v>0.12</v>
       </c>
       <c r="F4" t="n">
-        <v>0.93</v>
+        <v>0.44</v>
       </c>
       <c r="G4" t="n">
-        <v>0.66</v>
+        <v>0.055</v>
       </c>
       <c r="H4" t="n">
-        <v>0.81</v>
+        <v>0.86</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
       </c>
       <c r="J4" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="K4" t="n">
         <v>2.4</v>
       </c>
-      <c r="K4" t="n">
-        <v>5.4</v>
-      </c>
       <c r="L4" t="n">
-        <v>10.4</v>
+        <v>4.8</v>
       </c>
       <c r="M4" t="n">
-        <v>17.5</v>
+        <v>8.5</v>
       </c>
       <c r="N4" t="n">
-        <v>26.1</v>
+        <v>12.5</v>
       </c>
       <c r="O4" t="n">
-        <v>32.1</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="5">
@@ -672,46 +681,46 @@
         <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>13.4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>2.7</v>
+        <v>1.3</v>
       </c>
       <c r="D5" t="n">
-        <v>1.1</v>
+        <v>0.55</v>
       </c>
       <c r="E5" t="n">
-        <v>1.3</v>
+        <v>0.26</v>
       </c>
       <c r="F5" t="n">
-        <v>1.2</v>
+        <v>0.12</v>
       </c>
       <c r="G5" t="n">
-        <v>1.2</v>
+        <v>0.18</v>
       </c>
       <c r="H5" t="n">
-        <v>1.1</v>
+        <v>0.79</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="K5" t="n">
-        <v>5.5</v>
+        <v>2.9</v>
       </c>
       <c r="L5" t="n">
-        <v>9</v>
+        <v>5.9</v>
       </c>
       <c r="M5" t="n">
-        <v>16.2</v>
+        <v>9.6</v>
       </c>
       <c r="N5" t="n">
-        <v>22.3</v>
+        <v>15</v>
       </c>
       <c r="O5" t="n">
-        <v>29.8</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="6">
@@ -719,46 +728,46 @@
         <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>13.9</v>
+        <v>9.1</v>
       </c>
       <c r="C6" t="n">
-        <v>2.7</v>
+        <v>1.4</v>
       </c>
       <c r="D6" t="n">
-        <v>0.69</v>
+        <v>0.95</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0.13</v>
       </c>
       <c r="F6" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.000001</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I6" t="n">
         <v>1.2</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1.5</v>
-      </c>
       <c r="J6" t="n">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="K6" t="n">
-        <v>4.4</v>
+        <v>2.6</v>
       </c>
       <c r="L6" t="n">
-        <v>8.8</v>
+        <v>6.8</v>
       </c>
       <c r="M6" t="n">
-        <v>17.9</v>
+        <v>11.5</v>
       </c>
       <c r="N6" t="n">
-        <v>21.9</v>
+        <v>17.8</v>
       </c>
       <c r="O6" t="n">
-        <v>33.6</v>
+        <v>24.1</v>
       </c>
     </row>
     <row r="7">
@@ -766,46 +775,46 @@
         <v>20</v>
       </c>
       <c r="B7" t="n">
-        <v>13.9</v>
+        <v>11.9</v>
       </c>
       <c r="C7" t="n">
-        <v>3.7</v>
+        <v>1.2</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="E7" t="n">
-        <v>1.4</v>
+        <v>0.31</v>
       </c>
       <c r="F7" t="n">
-        <v>1.1</v>
+        <v>0.56</v>
       </c>
       <c r="G7" t="n">
-        <v>1.6</v>
+        <v>0.29</v>
       </c>
       <c r="H7" t="n">
-        <v>1.5</v>
+        <v>0.45</v>
       </c>
       <c r="I7" t="n">
-        <v>2.4</v>
+        <v>0.78</v>
       </c>
       <c r="J7" t="n">
-        <v>2.3</v>
+        <v>1.8</v>
       </c>
       <c r="K7" t="n">
-        <v>4</v>
+        <v>2.9</v>
       </c>
       <c r="L7" t="n">
-        <v>7.6</v>
+        <v>7.8</v>
       </c>
       <c r="M7" t="n">
-        <v>14.8</v>
+        <v>11</v>
       </c>
       <c r="N7" t="n">
-        <v>22.3</v>
+        <v>19.5</v>
       </c>
       <c r="O7" t="n">
-        <v>31.8</v>
+        <v>29.3</v>
       </c>
     </row>
     <row r="8">
@@ -813,46 +822,46 @@
         <v>21</v>
       </c>
       <c r="B8" t="n">
-        <v>10.9</v>
+        <v>9.8</v>
       </c>
       <c r="C8" t="n">
-        <v>2.3</v>
+        <v>1.4</v>
       </c>
       <c r="D8" t="n">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="E8" t="n">
-        <v>0.25</v>
+        <v>0.46</v>
       </c>
       <c r="F8" t="n">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="G8" t="n">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="H8" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="I8" t="n">
-        <v>1.1</v>
+        <v>1.4</v>
       </c>
       <c r="J8" t="n">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="K8" t="n">
-        <v>3.4</v>
+        <v>4.3</v>
       </c>
       <c r="L8" t="n">
-        <v>7.4</v>
+        <v>7.5</v>
       </c>
       <c r="M8" t="n">
-        <v>13</v>
+        <v>13.1</v>
       </c>
       <c r="N8" t="n">
-        <v>19.9</v>
+        <v>21.2</v>
       </c>
       <c r="O8" t="n">
-        <v>31.2</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="9">
@@ -860,46 +869,46 @@
         <v>22</v>
       </c>
       <c r="B9" t="n">
-        <v>9.8</v>
+        <v>10.9</v>
       </c>
       <c r="C9" t="n">
-        <v>1.4</v>
+        <v>2.3</v>
       </c>
       <c r="D9" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E9" t="n">
-        <v>0.46</v>
+        <v>0.25</v>
       </c>
       <c r="F9" t="n">
-        <v>0.17</v>
+        <v>0.21</v>
       </c>
       <c r="G9" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="H9" t="n">
-        <v>0.61</v>
+        <v>0.44</v>
       </c>
       <c r="I9" t="n">
-        <v>1.4</v>
+        <v>1.1</v>
       </c>
       <c r="J9" t="n">
-        <v>2.2</v>
+        <v>2.4</v>
       </c>
       <c r="K9" t="n">
-        <v>4.3</v>
+        <v>3.4</v>
       </c>
       <c r="L9" t="n">
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="M9" t="n">
-        <v>13.1</v>
+        <v>13</v>
       </c>
       <c r="N9" t="n">
-        <v>21.2</v>
+        <v>19.9</v>
       </c>
       <c r="O9" t="n">
-        <v>28.8</v>
+        <v>31.2</v>
       </c>
     </row>
     <row r="10">
@@ -907,46 +916,46 @@
         <v>23</v>
       </c>
       <c r="B10" t="n">
-        <v>11.9</v>
+        <v>13.9</v>
       </c>
       <c r="C10" t="n">
-        <v>1.2</v>
+        <v>3.7</v>
       </c>
       <c r="D10" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>0.31</v>
+        <v>1.4</v>
       </c>
       <c r="F10" t="n">
-        <v>0.56</v>
+        <v>1.1</v>
       </c>
       <c r="G10" t="n">
-        <v>0.29</v>
+        <v>1.6</v>
       </c>
       <c r="H10" t="n">
-        <v>0.45</v>
+        <v>1.5</v>
       </c>
       <c r="I10" t="n">
-        <v>0.78</v>
+        <v>2.4</v>
       </c>
       <c r="J10" t="n">
-        <v>1.8</v>
+        <v>2.3</v>
       </c>
       <c r="K10" t="n">
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="L10" t="n">
-        <v>7.8</v>
+        <v>7.6</v>
       </c>
       <c r="M10" t="n">
-        <v>11</v>
+        <v>14.8</v>
       </c>
       <c r="N10" t="n">
-        <v>19.5</v>
+        <v>22.3</v>
       </c>
       <c r="O10" t="n">
-        <v>29.3</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="11">
@@ -954,46 +963,46 @@
         <v>24</v>
       </c>
       <c r="B11" t="n">
-        <v>9.1</v>
+        <v>13.9</v>
       </c>
       <c r="C11" t="n">
-        <v>1.4</v>
+        <v>2.7</v>
       </c>
       <c r="D11" t="n">
-        <v>0.95</v>
+        <v>0.69</v>
       </c>
       <c r="E11" t="n">
-        <v>0.13</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.24</v>
+        <v>1.2</v>
       </c>
       <c r="G11" t="n">
-        <v>0.000001</v>
+        <v>0.78</v>
       </c>
       <c r="H11" t="n">
-        <v>0.45</v>
+        <v>0.67</v>
       </c>
       <c r="I11" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="J11" t="n">
-        <v>2.1</v>
+        <v>1.7</v>
       </c>
       <c r="K11" t="n">
-        <v>2.6</v>
+        <v>4.4</v>
       </c>
       <c r="L11" t="n">
-        <v>6.8</v>
+        <v>8.8</v>
       </c>
       <c r="M11" t="n">
-        <v>11.5</v>
+        <v>17.9</v>
       </c>
       <c r="N11" t="n">
-        <v>17.8</v>
+        <v>21.9</v>
       </c>
       <c r="O11" t="n">
-        <v>24.1</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="12">
@@ -1001,46 +1010,46 @@
         <v>25</v>
       </c>
       <c r="B12" t="n">
-        <v>7</v>
+        <v>13.4</v>
       </c>
       <c r="C12" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E12" t="n">
         <v>1.3</v>
       </c>
-      <c r="D12" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.26</v>
-      </c>
       <c r="F12" t="n">
-        <v>0.12</v>
+        <v>1.2</v>
       </c>
       <c r="G12" t="n">
-        <v>0.18</v>
+        <v>1.2</v>
       </c>
       <c r="H12" t="n">
-        <v>0.79</v>
+        <v>1.1</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="K12" t="n">
-        <v>2.9</v>
+        <v>5.5</v>
       </c>
       <c r="L12" t="n">
-        <v>5.9</v>
+        <v>9</v>
       </c>
       <c r="M12" t="n">
-        <v>9.6</v>
+        <v>16.2</v>
       </c>
       <c r="N12" t="n">
-        <v>15</v>
+        <v>22.3</v>
       </c>
       <c r="O12" t="n">
-        <v>23.3</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="13">
@@ -1048,46 +1057,46 @@
         <v>26</v>
       </c>
       <c r="B13" t="n">
-        <v>6.6</v>
+        <v>19</v>
       </c>
       <c r="C13" t="n">
-        <v>0.99</v>
+        <v>3.7</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5</v>
+        <v>1.1</v>
       </c>
       <c r="E13" t="n">
-        <v>0.12</v>
+        <v>0.84</v>
       </c>
       <c r="F13" t="n">
-        <v>0.44</v>
+        <v>0.93</v>
       </c>
       <c r="G13" t="n">
-        <v>0.055</v>
+        <v>0.66</v>
       </c>
       <c r="H13" t="n">
-        <v>0.86</v>
+        <v>0.81</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1.3</v>
+        <v>2.4</v>
       </c>
       <c r="K13" t="n">
-        <v>2.4</v>
+        <v>5.4</v>
       </c>
       <c r="L13" t="n">
-        <v>4.8</v>
+        <v>10.4</v>
       </c>
       <c r="M13" t="n">
-        <v>8.5</v>
+        <v>17.5</v>
       </c>
       <c r="N13" t="n">
-        <v>12.5</v>
+        <v>26.1</v>
       </c>
       <c r="O13" t="n">
-        <v>20.2</v>
+        <v>32.1</v>
       </c>
     </row>
     <row r="14">
@@ -1095,46 +1104,46 @@
         <v>27</v>
       </c>
       <c r="B14" t="n">
-        <v>6.5</v>
+        <v>21.1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.99</v>
+        <v>5.3</v>
       </c>
       <c r="D14" t="n">
-        <v>0.71</v>
+        <v>0.66</v>
       </c>
       <c r="E14" t="n">
-        <v>0.18</v>
+        <v>0.46</v>
       </c>
       <c r="F14" t="n">
-        <v>0.22</v>
+        <v>0.34</v>
       </c>
       <c r="G14" t="n">
-        <v>0.076</v>
+        <v>0.082</v>
       </c>
       <c r="H14" t="n">
-        <v>0.58</v>
+        <v>0.2</v>
       </c>
       <c r="I14" t="n">
-        <v>1.3</v>
+        <v>0.14</v>
       </c>
       <c r="J14" t="n">
         <v>1.2</v>
       </c>
       <c r="K14" t="n">
-        <v>2.6</v>
+        <v>5</v>
       </c>
       <c r="L14" t="n">
-        <v>3.8</v>
+        <v>11.3</v>
       </c>
       <c r="M14" t="n">
-        <v>6.5</v>
+        <v>17.9</v>
       </c>
       <c r="N14" t="n">
-        <v>12.7</v>
+        <v>25.4</v>
       </c>
       <c r="O14" t="n">
-        <v>20.3</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="15">
@@ -1142,46 +1151,46 @@
         <v>28</v>
       </c>
       <c r="B15" t="n">
-        <v>5.8</v>
+        <v>23.5</v>
       </c>
       <c r="C15" t="n">
-        <v>0.64</v>
+        <v>4.8</v>
       </c>
       <c r="D15" t="n">
-        <v>1.1</v>
+        <v>0.71</v>
       </c>
       <c r="E15" t="n">
-        <v>0.35</v>
+        <v>0.42</v>
       </c>
       <c r="F15" t="n">
-        <v>0.16</v>
+        <v>0.23</v>
       </c>
       <c r="G15" t="n">
-        <v>0.43</v>
+        <v>0.21</v>
       </c>
       <c r="H15" t="n">
-        <v>1.1</v>
+        <v>0.42</v>
       </c>
       <c r="I15" t="n">
-        <v>1.1</v>
+        <v>0.45</v>
       </c>
       <c r="J15" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="K15" t="n">
-        <v>1.3</v>
+        <v>4.8</v>
       </c>
       <c r="L15" t="n">
-        <v>3.2</v>
+        <v>9.8</v>
       </c>
       <c r="M15" t="n">
-        <v>5.2</v>
+        <v>17.9</v>
       </c>
       <c r="N15" t="n">
-        <v>10</v>
+        <v>23.4</v>
       </c>
       <c r="O15" t="n">
-        <v>16.8</v>
+        <v>33.1</v>
       </c>
     </row>
   </sheetData>
@@ -1191,12 +1200,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1260,6 +1269,22 @@
       </c>
       <c r="B8" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>